<commit_message>
Starting TransferCoordinator creation; minor FileHandler refactoring.
</commit_message>
<xml_diff>
--- a/WorkBot/main/backend/downloads/Russo Produce_IBProduce - Copy.xlsx
+++ b/WorkBot/main/backend/downloads/Russo Produce_IBProduce - Copy.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew\Desktop\Andrew\Projects\RandomStuff\WorkBot\main\backend\downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew\Desktop\Andrew\Projects\IthacaBakery\RandomStuff\WorkBot\main\backend\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9899941-9757-4BF3-BD0E-13F5B3E8786F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5ECB5EE-159B-424D-A760-6160353731DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -616,10 +625,10 @@
     <t>VPT</t>
   </si>
   <si>
+    <t>1 ea</t>
+  </si>
+  <si>
     <t>1 lb</t>
-  </si>
-  <si>
-    <t>1 ea</t>
   </si>
 </sst>
 </file>
@@ -678,7 +687,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -689,7 +698,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -972,14 +982,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75:XFD79"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1006,7 +1016,7 @@
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>151</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1014,13 +1024,16 @@
       </c>
       <c r="D2" s="3">
         <v>0.75</v>
+      </c>
+      <c r="G2" s="5">
+        <v>45871</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>153</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1034,7 +1047,7 @@
       <c r="A4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1048,25 +1061,28 @@
       <c r="A5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>177</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D5" s="3">
         <v>2.5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -1076,7 +1092,7 @@
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>152</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1090,21 +1106,24 @@
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>161</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D8" s="3">
         <v>5.5</v>
+      </c>
+      <c r="E8">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>149</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1118,11 +1137,11 @@
       <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>154</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D10" s="3">
         <v>12.5</v>
@@ -1132,7 +1151,7 @@
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>149</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1146,7 +1165,7 @@
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
         <v>132</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1158,187 +1177,190 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>129</v>
+        <v>68</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>187</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D13" s="3">
-        <v>15</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" t="s">
-        <v>190</v>
+        <v>0</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>120</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D14" s="3">
-        <v>16.5</v>
+        <v>16.850000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" t="s">
-        <v>187</v>
+        <v>44</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>163</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="D15" s="3">
-        <v>16.5</v>
+        <v>17.25</v>
+      </c>
+      <c r="E15">
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" t="s">
-        <v>120</v>
+        <v>9</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D16" s="3">
-        <v>16.850000000000001</v>
-      </c>
-      <c r="G16" s="5">
-        <v>45837</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" t="s">
-        <v>163</v>
+        <v>67</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>186</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="D17" s="3">
-        <v>17.25</v>
+        <v>18.5</v>
+      </c>
+      <c r="E17">
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" t="s">
-        <v>186</v>
+        <v>48</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>167</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D18" s="3">
         <v>18.5</v>
       </c>
-      <c r="E18">
-        <v>21.5</v>
-      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" t="s">
-        <v>167</v>
+        <v>5</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>125</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>81</v>
       </c>
       <c r="D19" s="3">
-        <v>18.5</v>
+        <v>18.850000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" t="s">
-        <v>125</v>
+        <v>39</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>158</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="D20" s="3">
-        <v>18.850000000000001</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" t="s">
-        <v>181</v>
+        <v>4</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>124</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D21" s="3">
-        <v>19</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22" t="s">
-        <v>178</v>
+        <v>43</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>162</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D22" s="3">
-        <v>19.850000000000001</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" t="s">
-        <v>124</v>
+        <v>71</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>190</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D23" s="3">
-        <v>20.5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" t="s">
-        <v>162</v>
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>143</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="D24" s="3">
-        <v>21</v>
+        <v>21.5</v>
+      </c>
+      <c r="E24">
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" t="s">
-        <v>158</v>
+        <v>41</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>160</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D25" s="3">
         <v>21.5</v>
@@ -1346,13 +1368,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" t="s">
-        <v>166</v>
+        <v>69</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>188</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="D26" s="3">
         <v>21.5</v>
@@ -1360,86 +1382,83 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" t="s">
-        <v>143</v>
+        <v>45</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>164</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D27" s="3">
-        <v>21.5</v>
+        <v>21.75</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" t="s">
-        <v>160</v>
+        <v>46</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>165</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D28" s="3">
-        <v>21.5</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29" t="s">
-        <v>188</v>
+        <v>26</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>146</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="D29" s="3">
-        <v>21.5</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" t="s">
-        <v>164</v>
+        <v>24</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>144</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D30" s="3">
-        <v>21.75</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" t="s">
-        <v>148</v>
+        <v>20</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>140</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D31" s="3">
-        <v>21.85</v>
-      </c>
-      <c r="E31">
-        <v>23.85</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" t="s">
-        <v>165</v>
+        <v>64</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>183</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="D32" s="3">
         <v>22.5</v>
@@ -1447,13 +1466,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" t="s">
-        <v>146</v>
+        <v>60</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>179</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="D33" s="3">
         <v>22.5</v>
@@ -1461,282 +1480,291 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B34" t="s">
-        <v>144</v>
+        <v>50</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>169</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D34" s="3">
-        <v>22.5</v>
+        <v>22.85</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35" t="s">
-        <v>140</v>
+        <v>28</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>148</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D35" s="3">
-        <v>22.5</v>
+        <v>23.85</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B36" t="s">
-        <v>134</v>
+        <v>59</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>178</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="D36" s="3">
-        <v>22.5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B37" t="s">
-        <v>183</v>
+        <v>47</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>166</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="D37" s="3">
-        <v>22.5</v>
+        <v>24</v>
+      </c>
+      <c r="E37">
+        <v>21.85</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B38" t="s">
-        <v>179</v>
+        <v>30</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>150</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="D38" s="3">
-        <v>22.5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B39" t="s">
-        <v>169</v>
+        <v>14</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>134</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D39" s="3">
-        <v>22.85</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>56</v>
+      <c r="A40" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="D40" s="3">
-        <v>23.5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B41" t="s">
-        <v>176</v>
+        <v>40</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>159</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="D41" s="3">
-        <v>23.5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B42" t="s">
-        <v>150</v>
+        <v>52</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>171</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="D42" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B43" t="s">
-        <v>168</v>
+        <v>113</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>191</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="D43" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B44" t="s">
-        <v>171</v>
+        <v>13</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>133</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D44" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B45" t="s">
-        <v>191</v>
+        <v>6</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>126</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="D45" s="3">
-        <v>25</v>
+        <v>26.5</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B46" t="s">
-        <v>126</v>
+        <v>25</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>145</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D46" s="3">
-        <v>25.5</v>
-      </c>
-      <c r="E46">
-        <v>27.5</v>
+        <v>26.85</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B47" t="s">
-        <v>159</v>
+        <v>27</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>147</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D47" s="3">
-        <v>26.5</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B48" t="s">
-        <v>145</v>
+        <v>63</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>182</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D48" s="3">
-        <v>26.85</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B49" t="s">
-        <v>130</v>
+        <v>54</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>173</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="D49" s="3">
-        <v>27.5</v>
+        <v>28.5</v>
+      </c>
+      <c r="E49">
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B50" t="s">
-        <v>189</v>
+        <v>55</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>174</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="D50" s="3">
-        <v>27.5</v>
+        <v>28.5</v>
+      </c>
+      <c r="E50">
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B51" t="s">
-        <v>182</v>
+        <v>70</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>189</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D51" s="3">
-        <v>27.5</v>
+        <v>28.5</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B52" t="s">
-        <v>173</v>
+        <v>11</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>131</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="D52" s="3">
         <v>28.5</v>
       </c>
+      <c r="E52">
+        <v>22.5</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B53" t="s">
-        <v>174</v>
+        <v>62</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>181</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="D53" s="3">
         <v>28.5</v>
@@ -1744,23 +1772,23 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B54" t="s">
-        <v>131</v>
+        <v>10</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D54" s="3">
-        <v>28.5</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="6" t="s">
         <v>139</v>
       </c>
       <c r="C55" s="3" t="s">
@@ -1774,7 +1802,7 @@
       <c r="A56" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="6" t="s">
         <v>184</v>
       </c>
       <c r="C56" s="3" t="s">
@@ -1786,100 +1814,97 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B57" t="s">
-        <v>133</v>
+        <v>18</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D57" s="3">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B58" t="s">
-        <v>138</v>
+        <v>2</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>122</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>116</v>
+        <v>79</v>
       </c>
       <c r="D58" s="3">
-        <v>32</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B59" t="s">
-        <v>122</v>
+        <v>22</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>142</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="D59" s="3">
-        <v>32.5</v>
+        <v>34.5</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B60" t="s">
-        <v>147</v>
+        <v>7</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="D60" s="3">
-        <v>34.5</v>
-      </c>
-      <c r="E60">
-        <v>36.5</v>
+        <v>35.85</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B61" t="s">
-        <v>142</v>
+        <v>37</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>156</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D61" s="3">
-        <v>34.5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B62" t="s">
-        <v>127</v>
+      <c r="A62" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>175</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D62" s="3">
-        <v>35.85</v>
+        <v>36</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B63" t="s">
-        <v>157</v>
+        <v>57</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>176</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D63" s="3">
         <v>36</v>
@@ -1887,68 +1912,65 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B64" t="s">
-        <v>156</v>
+        <v>3</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>123</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="D64" s="3">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B65" t="s">
-        <v>123</v>
+        <v>1</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>119</v>
+        <v>78</v>
       </c>
       <c r="D65" s="3">
-        <v>37.5</v>
-      </c>
-      <c r="F65" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="6" t="s">
         <v>137</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>88</v>
       </c>
       <c r="D66" s="3">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B67" t="s">
-        <v>121</v>
+        <v>16</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="D67" s="3">
-        <v>39.5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="6" t="s">
         <v>170</v>
       </c>
       <c r="C68" s="3" t="s">
@@ -1958,11 +1980,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="6" t="s">
         <v>155</v>
       </c>
       <c r="C69" s="3" t="s">
@@ -1972,25 +1994,28 @@
         <v>42.5</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B70" t="s">
-        <v>128</v>
+        <v>38</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>157</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="D70" s="3">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+        <v>42.5</v>
+      </c>
+      <c r="E70">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="6" t="s">
         <v>141</v>
       </c>
       <c r="C71" s="3">
@@ -1999,51 +2024,54 @@
       <c r="D71" s="3">
         <v>48</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E71">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D72" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D73" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B74" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="C74" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D72" s="3">
+      <c r="D74" s="3">
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B73" t="s">
-        <v>136</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D73" s="3">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B74" t="s">
-        <v>172</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D74" s="3">
-        <v>58</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G74">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D74">
     <sortCondition ref="D2:D74"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished selenium session context manager handler
</commit_message>
<xml_diff>
--- a/WorkBot/main/backend/downloads/Russo Produce_IBProduce - Copy.xlsx
+++ b/WorkBot/main/backend/downloads/Russo Produce_IBProduce - Copy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew\Desktop\Andrew\Projects\IthacaBakery\RandomStuff\WorkBot\main\backend\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5ECB5EE-159B-424D-A760-6160353731DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923B64B1-A772-4404-B10C-AA2B5F0C6DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="196">
   <si>
     <t>Alfalfa Sprouts</t>
   </si>
@@ -625,10 +625,16 @@
     <t>VPT</t>
   </si>
   <si>
+    <t>SKU</t>
+  </si>
+  <si>
     <t>1 ea</t>
   </si>
   <si>
     <t>1 lb</t>
+  </si>
+  <si>
+    <t>1bu</t>
   </si>
 </sst>
 </file>
@@ -687,7 +693,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -698,8 +704,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -982,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,7 +1003,9 @@
       <c r="A1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="3" t="s">
+        <v>192</v>
+      </c>
       <c r="C1" s="3" t="s">
         <v>73</v>
       </c>
@@ -1014,27 +1021,27 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>99</v>
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="3">
+        <v>30</v>
       </c>
       <c r="D2" s="3">
-        <v>0.75</v>
+        <v>48</v>
       </c>
       <c r="G2" s="5">
-        <v>45871</v>
+        <v>45885</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>153</v>
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>151</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>99</v>
@@ -1047,7 +1054,7 @@
       <c r="A4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1059,876 +1066,864 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>177</v>
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>162</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>193</v>
+        <v>105</v>
       </c>
       <c r="D5" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>119</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>135</v>
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>165</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>193</v>
+        <v>105</v>
       </c>
       <c r="D6" s="3">
-        <v>3</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>152</v>
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>173</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D7" s="3">
-        <v>3.5</v>
+        <v>28.5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>161</v>
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>174</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>192</v>
+        <v>105</v>
       </c>
       <c r="D8" s="3">
-        <v>5.5</v>
-      </c>
-      <c r="E8">
-        <v>24</v>
+        <v>28.5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>149</v>
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
+        <v>178</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="D9" s="3">
-        <v>12.5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>154</v>
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>155</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>193</v>
+        <v>100</v>
       </c>
       <c r="D10" s="3">
-        <v>12.5</v>
+        <v>42.5</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>149</v>
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>157</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D11" s="3">
-        <v>13.85</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>132</v>
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>123</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="D12" s="3">
-        <v>14</v>
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>187</v>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>132</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D13" s="3">
-        <v>16.5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>120</v>
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
+        <v>190</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D14" s="3">
-        <v>16.850000000000001</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>163</v>
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>130</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="D15" s="3">
-        <v>17.25</v>
-      </c>
-      <c r="E15">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>129</v>
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>156</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D16" s="3">
-        <v>17.5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>186</v>
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>147</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="D17" s="3">
-        <v>18.5</v>
+        <v>28.5</v>
       </c>
       <c r="E17">
-        <v>15</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>167</v>
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>146</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="D18" s="3">
-        <v>18.5</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>125</v>
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>137</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="D19" s="3">
-        <v>18.850000000000001</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>158</v>
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>136</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="D20" s="3">
-        <v>19.5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>124</v>
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>145</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="D21" s="3">
-        <v>20.5</v>
+        <v>26.85</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>162</v>
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>139</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="D22" s="3">
-        <v>21</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>190</v>
+        <v>68</v>
+      </c>
+      <c r="B23" t="s">
+        <v>187</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D23" s="3">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>143</v>
+        <v>67</v>
+      </c>
+      <c r="B24" t="s">
+        <v>186</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="D24" s="3">
-        <v>21.5</v>
-      </c>
-      <c r="E24">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>160</v>
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>126</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="D25" s="3">
-        <v>21.5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>188</v>
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>171</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D26" s="3">
-        <v>21.5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>164</v>
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>144</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D27" s="3">
-        <v>21.75</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>165</v>
+        <v>13</v>
+      </c>
+      <c r="B28" t="s">
+        <v>133</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="D28" s="3">
-        <v>22.5</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>146</v>
+        <v>9</v>
+      </c>
+      <c r="B29" t="s">
+        <v>129</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="D29" s="3">
-        <v>22.5</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>144</v>
+        <v>48</v>
+      </c>
+      <c r="B30" t="s">
+        <v>167</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="D30" s="3">
-        <v>22.5</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>140</v>
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>125</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D31" s="3">
-        <v>22.5</v>
+        <v>18.850000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>64</v>
+      <c r="A32" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D32" s="3">
         <v>22.5</v>
       </c>
+      <c r="E32">
+        <v>21</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>179</v>
+        <v>57</v>
+      </c>
+      <c r="B33" t="s">
+        <v>176</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="D33" s="3">
         <v>22.5</v>
       </c>
+      <c r="E33">
+        <v>21</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>169</v>
+        <v>70</v>
+      </c>
+      <c r="B34" t="s">
+        <v>189</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D34" s="3">
-        <v>22.85</v>
+        <v>28.5</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>148</v>
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>128</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="D35" s="3">
-        <v>23.85</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>178</v>
+        <v>113</v>
+      </c>
+      <c r="B36" t="s">
+        <v>191</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="D36" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>166</v>
+        <v>18</v>
+      </c>
+      <c r="B37" t="s">
+        <v>138</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="D37" s="3">
-        <v>24</v>
-      </c>
-      <c r="E37">
-        <v>21.85</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>150</v>
+        <v>31</v>
+      </c>
+      <c r="B38" t="s">
+        <v>149</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D38" s="3">
-        <v>24</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>134</v>
+        <v>29</v>
+      </c>
+      <c r="B39" t="s">
+        <v>149</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="D39" s="3">
-        <v>24</v>
+        <v>13.85</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>168</v>
+        <v>45</v>
+      </c>
+      <c r="B40" t="s">
+        <v>164</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D40" s="3">
-        <v>24</v>
+        <v>21.75</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>159</v>
+        <v>11</v>
+      </c>
+      <c r="B41" t="s">
+        <v>131</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="D41" s="3">
-        <v>24</v>
+        <v>28.5</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>171</v>
+        <v>61</v>
+      </c>
+      <c r="B42" t="s">
+        <v>180</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="D42" s="3">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>191</v>
+        <v>22</v>
+      </c>
+      <c r="B43" t="s">
+        <v>142</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="D43" s="3">
-        <v>25</v>
+        <v>34.5</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>133</v>
+        <v>39</v>
+      </c>
+      <c r="B44" t="s">
+        <v>158</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D44" s="3">
-        <v>26</v>
+        <v>18</v>
+      </c>
+      <c r="E44">
+        <v>16.5</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>126</v>
+        <v>20</v>
+      </c>
+      <c r="B45" t="s">
+        <v>140</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="D45" s="3">
-        <v>26.5</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>145</v>
+        <v>47</v>
+      </c>
+      <c r="B46" t="s">
+        <v>166</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="D46" s="3">
-        <v>26.85</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>147</v>
+        <v>30</v>
+      </c>
+      <c r="B47" t="s">
+        <v>150</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D47" s="3">
-        <v>27.5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" t="s">
+        <v>143</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" s="3">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" t="s">
+        <v>124</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" s="3">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" t="s">
+        <v>184</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D50" s="3">
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" t="s">
+        <v>172</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D51" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" t="s">
+        <v>160</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D52" s="3">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B53" t="s">
+        <v>163</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D53" s="3">
+        <v>17.25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" t="s">
+        <v>134</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D54" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B55" t="s">
+        <v>168</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D55" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B56" t="s">
+        <v>183</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D56" s="3">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B57" t="s">
+        <v>169</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D57" s="3">
+        <v>22.85</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58" t="s">
+        <v>181</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D58" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B59" t="s">
         <v>182</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C59" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D59" s="3">
         <v>27.5</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D49" s="3">
-        <v>28.5</v>
-      </c>
-      <c r="E49">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D50" s="3">
-        <v>28.5</v>
-      </c>
-      <c r="E50">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D51" s="3">
-        <v>28.5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D52" s="3">
-        <v>28.5</v>
-      </c>
-      <c r="E52">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" t="s">
+        <v>120</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D60" s="3">
+        <v>16.850000000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D61" s="3">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B62" t="s">
+        <v>148</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D62" s="3">
+        <v>21.85</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" t="s">
+        <v>127</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D63" s="3">
+        <v>35.85</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B64" t="s">
+        <v>179</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D64" s="3">
         <v>22.5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D53" s="3">
-        <v>28.5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D54" s="3">
-        <v>29.5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D55" s="3">
-        <v>29.5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D56" s="3">
-        <v>29.5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D57" s="3">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D58" s="3">
-        <v>32.5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D59" s="3">
-        <v>34.5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D60" s="3">
-        <v>35.85</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D61" s="3">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D62" s="3">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D63" s="3">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D64" s="3">
-        <v>37.5</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="B65" t="s">
         <v>121</v>
       </c>
       <c r="C65" s="3" t="s">
@@ -1940,27 +1935,30 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>137</v>
+        <v>69</v>
+      </c>
+      <c r="B66" t="s">
+        <v>188</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="D66" s="3">
-        <v>40</v>
+        <v>21.5</v>
+      </c>
+      <c r="E66">
+        <v>22.5</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>136</v>
+        <v>51</v>
+      </c>
+      <c r="B67" t="s">
+        <v>170</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="D67" s="3">
         <v>42</v>
@@ -1968,111 +1966,108 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>170</v>
+        <v>40</v>
+      </c>
+      <c r="B68" t="s">
+        <v>159</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="D68" s="3">
-        <v>42</v>
+        <v>22.5</v>
+      </c>
+      <c r="E68">
+        <v>23.5</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>155</v>
+        <v>34</v>
+      </c>
+      <c r="B69" t="s">
+        <v>153</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D69" s="3">
-        <v>42.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>157</v>
+        <v>33</v>
+      </c>
+      <c r="B70" t="s">
+        <v>152</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>101</v>
+        <v>195</v>
       </c>
       <c r="D70" s="3">
-        <v>42.5</v>
-      </c>
-      <c r="E70">
-        <v>26</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="C71" s="3">
-        <v>30</v>
+        <v>58</v>
+      </c>
+      <c r="B71" t="s">
+        <v>177</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="D71" s="3">
-        <v>48</v>
-      </c>
-      <c r="E71">
-        <v>26</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>128</v>
+        <v>15</v>
+      </c>
+      <c r="B72" t="s">
+        <v>135</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>81</v>
+        <v>194</v>
       </c>
       <c r="D72" s="3">
-        <v>52</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>172</v>
+        <v>35</v>
+      </c>
+      <c r="B73" t="s">
+        <v>154</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>108</v>
+        <v>194</v>
       </c>
       <c r="D73" s="3">
-        <v>52</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B74" s="6" t="s">
-        <v>180</v>
+        <v>42</v>
+      </c>
+      <c r="B74" t="s">
+        <v>161</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>86</v>
+        <v>193</v>
       </c>
       <c r="D74" s="3">
-        <v>55</v>
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D74">
-    <sortCondition ref="D2:D74"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F89">
+    <sortCondition ref="C2:C89"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>